<commit_message>
ng: update prestop form
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Nigeria/ng_oncho_prestop_1_site_202208.xlsx
+++ b/ONCHO/Impact Assessments/Nigeria/ng_oncho_prestop_1_site_202208.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="163">
   <si>
     <t>type</t>
   </si>
@@ -382,9 +382,15 @@
     <t>Karasuwa</t>
   </si>
   <si>
+    <t>Nangere</t>
+  </si>
+  <si>
     <t>Nguru</t>
   </si>
   <si>
+    <t>Potiskum</t>
+  </si>
+  <si>
     <t>Tarmuwa</t>
   </si>
   <si>
@@ -448,12 +454,24 @@
     <t>Garunguna</t>
   </si>
   <si>
+    <t>Garin Gada</t>
+  </si>
+  <si>
+    <t>Tarajim</t>
+  </si>
+  <si>
     <t>Dabule</t>
   </si>
   <si>
     <t>Yamdugu</t>
   </si>
   <si>
+    <t>Danchiwa</t>
+  </si>
+  <si>
+    <t>Garin Zaniwa</t>
+  </si>
+  <si>
     <t>Muli</t>
   </si>
   <si>
@@ -472,10 +490,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Aug 2022) ONCHO PreStop - 1. Site Form</t>
-  </si>
-  <si>
-    <t>ng_oncho_prestop_1_site_202208</t>
+    <t>(Aug 2022) ONCHO PreStop - 1. Site Form V2</t>
+  </si>
+  <si>
+    <t>ng_oncho_prestop_1_site_202208_v2</t>
   </si>
   <si>
     <t>English</t>
@@ -495,10 +513,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -561,81 +579,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -654,12 +597,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -668,7 +620,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -683,7 +658,50 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -704,13 +722,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,7 +746,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,79 +788,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,19 +806,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -848,19 +824,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,19 +890,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -953,45 +971,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1021,11 +1000,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1040,145 +1025,178 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1188,7 +1206,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1212,6 +1230,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1562,7 +1584,7 @@
   <sheetPr/>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -1588,43 +1610,43 @@
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="1" ht="18" spans="1:13">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="22" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1632,74 +1654,74 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:12">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16" t="s">
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1707,24 +1729,24 @@
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="18" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16" t="s">
+      <c r="D5" s="18"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16" t="s">
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1732,66 +1754,66 @@
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="18" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="14" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16" t="s">
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16" t="s">
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" s="14" customFormat="1" ht="15.75" customHeight="1" spans="1:13">
+    <row r="7" s="16" customFormat="1" ht="15.75" customHeight="1" spans="1:13">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="J8" s="16" t="s">
+      <c r="D8" s="19"/>
+      <c r="J8" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1802,12 +1824,12 @@
       <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="H9" s="14"/>
-      <c r="J9" s="16" t="s">
+      <c r="D9" s="19"/>
+      <c r="H9" s="16"/>
+      <c r="J9" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1821,9 +1843,9 @@
       <c r="C10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="H10" s="14"/>
-      <c r="J10" s="16" t="s">
+      <c r="D10" s="19"/>
+      <c r="H10" s="16"/>
+      <c r="J10" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1840,7 +1862,7 @@
       <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1851,10 +1873,10 @@
       <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1868,7 +1890,7 @@
       <c r="C13" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1882,7 +1904,7 @@
       <c r="C14" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1896,7 +1918,7 @@
       <c r="C15" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1910,7 +1932,7 @@
       <c r="C16" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="16" t="s">
+      <c r="J16" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1924,7 +1946,7 @@
       <c r="C17" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="J17" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1941,7 +1963,7 @@
       <c r="H18" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1958,7 +1980,7 @@
       <c r="H19" t="s">
         <v>67</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J19" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1981,7 +2003,7 @@
       <c r="H20" t="s">
         <v>67</v>
       </c>
-      <c r="J20" s="16" t="s">
+      <c r="J20" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1998,7 +2020,7 @@
       <c r="I21" t="s">
         <v>78</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="J21" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2017,7 +2039,7 @@
       <c r="A23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="19" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2025,7 +2047,7 @@
       <c r="A24" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="19" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2039,12 +2061,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -2068,7 +2090,7 @@
       <c r="D1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="15" t="s">
         <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2532,32 +2554,32 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="37" s="4" customFormat="1" spans="1:4">
+      <c r="A37" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C37" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D37" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" s="4" customFormat="1" spans="1:4">
+      <c r="A38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C38" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E39" t="s">
-        <v>113</v>
+      <c r="D38" s="7" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2571,7 +2593,7 @@
         <v>126</v>
       </c>
       <c r="E40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2585,7 +2607,7 @@
         <v>127</v>
       </c>
       <c r="E41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2599,7 +2621,7 @@
         <v>128</v>
       </c>
       <c r="E42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2627,7 +2649,7 @@
         <v>130</v>
       </c>
       <c r="E44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2641,7 +2663,7 @@
         <v>131</v>
       </c>
       <c r="E45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2697,7 +2719,7 @@
         <v>135</v>
       </c>
       <c r="E49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2711,7 +2733,7 @@
         <v>136</v>
       </c>
       <c r="E50" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2725,7 +2747,7 @@
         <v>137</v>
       </c>
       <c r="E51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2739,7 +2761,7 @@
         <v>138</v>
       </c>
       <c r="E52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2753,7 +2775,7 @@
         <v>139</v>
       </c>
       <c r="E53" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2767,7 +2789,7 @@
         <v>140</v>
       </c>
       <c r="E54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2795,7 +2817,7 @@
         <v>142</v>
       </c>
       <c r="E56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2809,7 +2831,7 @@
         <v>143</v>
       </c>
       <c r="E57" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2823,7 +2845,7 @@
         <v>144</v>
       </c>
       <c r="E58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2837,7 +2859,7 @@
         <v>145</v>
       </c>
       <c r="E59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2851,334 +2873,475 @@
         <v>146</v>
       </c>
       <c r="E60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>147</v>
+      </c>
+      <c r="C61" t="s">
+        <v>147</v>
+      </c>
+      <c r="E61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" t="s">
+        <v>148</v>
+      </c>
+      <c r="E62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E63" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
-        <v>147</v>
-      </c>
-      <c r="B62">
-        <v>101</v>
-      </c>
-      <c r="C62">
-        <v>101</v>
-      </c>
-      <c r="F62" t="s">
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" t="s">
+        <v>150</v>
+      </c>
+      <c r="C64" t="s">
+        <v>150</v>
+      </c>
+      <c r="E64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" t="s">
+        <v>151</v>
+      </c>
+      <c r="E65" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
-        <v>147</v>
-      </c>
-      <c r="B63">
-        <v>102</v>
-      </c>
-      <c r="C63">
-        <v>102</v>
-      </c>
-      <c r="F63" t="s">
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" t="s">
+        <v>152</v>
+      </c>
+      <c r="C66" t="s">
+        <v>152</v>
+      </c>
+      <c r="E66" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>147</v>
-      </c>
-      <c r="B64">
-        <v>103</v>
-      </c>
-      <c r="C64">
-        <v>103</v>
-      </c>
-      <c r="F64" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>147</v>
-      </c>
-      <c r="B65">
-        <v>104</v>
-      </c>
-      <c r="C65">
-        <v>104</v>
-      </c>
-      <c r="F65" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>147</v>
-      </c>
-      <c r="B66">
-        <v>105</v>
-      </c>
-      <c r="C66">
-        <v>105</v>
-      </c>
-      <c r="F66" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
-        <v>147</v>
-      </c>
-      <c r="B67">
-        <v>106</v>
-      </c>
-      <c r="C67">
-        <v>106</v>
-      </c>
-      <c r="F67" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B68">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C68">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F68" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B69">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C69">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F69" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B70">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C70">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F70" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B71">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C71">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F71" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B72">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C72">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F72" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B73">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C73">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F73" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B74">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C74">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F74" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B75">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C75">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F75" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B76">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C76">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F76" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B77">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C77">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F77" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B78">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C78">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F78" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B79">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C79">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F79" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B80">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C80">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F80" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B81">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C81">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F81" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B82">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C82">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F82" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B83">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C83">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F83" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
+        <v>153</v>
+      </c>
+      <c r="B84">
+        <v>117</v>
+      </c>
+      <c r="C84">
+        <v>117</v>
+      </c>
+      <c r="F84" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>153</v>
+      </c>
+      <c r="B85">
+        <v>118</v>
+      </c>
+      <c r="C85">
+        <v>118</v>
+      </c>
+      <c r="F85" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>153</v>
+      </c>
+      <c r="B86">
+        <v>119</v>
+      </c>
+      <c r="C86">
+        <v>119</v>
+      </c>
+      <c r="F86" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>153</v>
+      </c>
+      <c r="B87">
+        <v>120</v>
+      </c>
+      <c r="C87">
+        <v>120</v>
+      </c>
+      <c r="F87" t="s">
         <v>147</v>
       </c>
-      <c r="B84">
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>153</v>
+      </c>
+      <c r="B88">
+        <v>121</v>
+      </c>
+      <c r="C88">
+        <v>121</v>
+      </c>
+      <c r="F88" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>153</v>
+      </c>
+      <c r="B89">
+        <v>122</v>
+      </c>
+      <c r="C89">
+        <v>122</v>
+      </c>
+      <c r="F89" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90">
         <v>123</v>
       </c>
-      <c r="C84">
+      <c r="C90">
         <v>123</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F90" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>153</v>
+      </c>
+      <c r="B91">
+        <v>124</v>
+      </c>
+      <c r="C91">
+        <v>124</v>
+      </c>
+      <c r="F91" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>153</v>
+      </c>
+      <c r="B92">
+        <v>125</v>
+      </c>
+      <c r="C92">
+        <v>125</v>
+      </c>
+      <c r="F92" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" t="s">
+        <v>153</v>
+      </c>
+      <c r="B93">
+        <v>126</v>
+      </c>
+      <c r="C93">
+        <v>126</v>
+      </c>
+      <c r="F93" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" t="s">
+        <v>153</v>
+      </c>
+      <c r="B94">
+        <v>127</v>
+      </c>
+      <c r="C94">
+        <v>127</v>
+      </c>
+      <c r="F94" t="s">
         <v>146</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A10:E46">
-    <sortCondition ref="B10:B46"/>
+  <sortState ref="A40:E66">
+    <sortCondition ref="A40:A66"/>
+    <sortCondition ref="E40:E66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -3191,35 +3354,35 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="46.1259259259259" customWidth="1"/>
-    <col min="2" max="2" width="30.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3252,21 +3415,19 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1"/>
-      <c r="F1"/>
+        <v>162</v>
+      </c>
       <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:8">
@@ -3277,13 +3438,11 @@
         <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D2">
         <v>101</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" t="s">
         <v>111</v>
       </c>
@@ -3299,13 +3458,11 @@
         <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D3">
         <v>102</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" t="s">
         <v>111</v>
       </c>
@@ -3321,13 +3478,11 @@
         <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D4">
         <v>103</v>
       </c>
-      <c r="E4"/>
-      <c r="F4"/>
       <c r="G4" t="s">
         <v>111</v>
       </c>
@@ -3343,13 +3498,11 @@
         <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D5">
         <v>104</v>
       </c>
-      <c r="E5"/>
-      <c r="F5"/>
       <c r="G5" t="s">
         <v>111</v>
       </c>
@@ -3365,13 +3518,11 @@
         <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D6">
         <v>105</v>
       </c>
-      <c r="E6"/>
-      <c r="F6"/>
       <c r="G6" t="s">
         <v>111</v>
       </c>
@@ -3387,13 +3538,11 @@
         <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D7">
         <v>106</v>
       </c>
-      <c r="E7"/>
-      <c r="F7"/>
       <c r="G7" t="s">
         <v>111</v>
       </c>
@@ -3409,13 +3558,11 @@
         <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D8">
         <v>107</v>
       </c>
-      <c r="E8"/>
-      <c r="F8"/>
       <c r="G8" t="s">
         <v>111</v>
       </c>
@@ -3431,13 +3578,11 @@
         <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D9">
         <v>108</v>
       </c>
-      <c r="E9"/>
-      <c r="F9"/>
       <c r="G9" t="s">
         <v>111</v>
       </c>
@@ -3453,13 +3598,11 @@
         <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D10">
         <v>109</v>
       </c>
-      <c r="E10"/>
-      <c r="F10"/>
       <c r="G10" t="s">
         <v>111</v>
       </c>
@@ -3475,18 +3618,16 @@
         <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D11">
         <v>110</v>
       </c>
-      <c r="E11"/>
-      <c r="F11"/>
       <c r="G11" t="s">
         <v>111</v>
       </c>
       <c r="H11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:8">
@@ -3497,18 +3638,16 @@
         <v>115</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D12">
         <v>111</v>
       </c>
-      <c r="E12"/>
-      <c r="F12"/>
       <c r="G12" t="s">
         <v>111</v>
       </c>
       <c r="H12" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:8">
@@ -3519,18 +3658,16 @@
         <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D13">
         <v>112</v>
       </c>
-      <c r="E13"/>
-      <c r="F13"/>
       <c r="G13" t="s">
         <v>111</v>
       </c>
       <c r="H13" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:4">
@@ -3541,7 +3678,7 @@
         <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D14">
         <v>113</v>
@@ -3555,7 +3692,7 @@
         <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D15">
         <v>114</v>
@@ -3569,7 +3706,7 @@
         <v>118</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D16">
         <v>115</v>
@@ -3583,7 +3720,7 @@
         <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D17">
         <v>116</v>
@@ -3597,7 +3734,7 @@
         <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D18">
         <v>117</v>
@@ -3611,7 +3748,7 @@
         <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D19">
         <v>118</v>
@@ -3625,7 +3762,7 @@
         <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D20">
         <v>119</v>
@@ -3636,10 +3773,10 @@
         <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D21">
         <v>120</v>
@@ -3650,10 +3787,10 @@
         <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D22">
         <v>121</v>
@@ -3664,10 +3801,10 @@
         <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D23">
         <v>122</v>
@@ -3678,10 +3815,10 @@
         <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C24" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D24">
         <v>123</v>

</xml_diff>